<commit_message>
Extending to FTSE100 csv file and any csv file
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>2023-01-28 13:10:16</t>
+          <t>2023-01-28 13:27:19</t>
         </is>
       </c>
     </row>
@@ -511,93 +511,93 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ADBE</t>
+          <t>CUK</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>370.71</v>
+        <v>9.949999999999999</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>0.005942857142857143</v>
+        <v>0.01845714285714286</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AOS</t>
+          <t>BLND</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>60.36</v>
+        <v>1.61</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>0.003195238095238096</v>
+        <v>0.01822857142857143</v>
       </c>
       <c r="D6" s="4" t="n">
         <v>0.5714285714285714</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ACN</t>
+          <t>AAL</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>277.27</v>
+        <v>16.43</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>0.002619047619047618</v>
+        <v>0.01418095238095238</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>0.5238095238095237</v>
+        <v>0.7142857142857144</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ABT</t>
+          <t>IHG</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>109.95</v>
+        <v>71.73999999999999</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>0.0009904761904761909</v>
+        <v>0.01055714285714286</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.8095238095238098</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>AAP</t>
+          <t>WPP</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>147.44</v>
+        <v>58.84</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>0.0007952380952380958</v>
+        <v>0.00917142857142857</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>0.4761904761904762</v>
+        <v>0.7619047619047621</v>
       </c>
       <c r="E9" t="n">
         <v>2</v>
@@ -606,162 +606,782 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ATVI</t>
+          <t>CRH</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>76.61</v>
+        <v>46.47</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>0.0003952380952380955</v>
+        <v>0.008033333333333333</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MMM</t>
+          <t>EVR</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>115.25</v>
+        <v>127.76</v>
       </c>
       <c r="C11" s="4" t="n">
-        <v>-0.000980952380952381</v>
+        <v>0.007733333333333334</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>0.6190476190476191</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ABBV</t>
+          <t>SVT</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>146.28</v>
+        <v>11.9</v>
       </c>
       <c r="C12" s="4" t="n">
-        <v>-0.004842857142857143</v>
+        <v>0.007172222222222223</v>
       </c>
       <c r="D12" s="4" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.5555555555555557</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>HL</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>6.24</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>0.007133333333333333</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>0.6190476190476191</v>
+      </c>
+      <c r="E13" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>VOD</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>11.61</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>0.00699047619047619</v>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>0.4761904761904762</v>
+      </c>
+      <c r="E14" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>IAG</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>0.006304761904761904</v>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>0.5238095238095237</v>
+      </c>
+      <c r="E15" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>GFS</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>59.24</v>
+      </c>
+      <c r="C16" s="4" t="n">
+        <v>0.006285714285714285</v>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>0.6190476190476191</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>RIO</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>79.61</v>
+      </c>
+      <c r="C17" s="4" t="n">
+        <v>0.005776190476190476</v>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>0.7142857142857144</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>BA</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>211.17</v>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>0.005580952380952382</v>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ADN</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>0.005123809523809524</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="E19" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CPG</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>7.48</v>
+      </c>
+      <c r="C20" s="4" t="n">
+        <v>0.004471428571428572</v>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>0.6190476190476191</v>
+      </c>
+      <c r="E20" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>BSY</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>39.16</v>
+      </c>
+      <c r="C21" s="4" t="n">
+        <v>0.004380952380952381</v>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>REX</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>31.71</v>
+      </c>
+      <c r="C22" s="4" t="n">
+        <v>0.0038</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>0.6190476190476191</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>LAND</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>19.42</v>
+      </c>
+      <c r="C23" s="4" t="n">
+        <v>0.003623809523809524</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="E23" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>MRO</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>28.31</v>
+      </c>
+      <c r="C24" s="4" t="n">
+        <v>0.003180952380952381</v>
+      </c>
+      <c r="D24" s="4" t="n">
+        <v>0.6190476190476191</v>
+      </c>
+      <c r="E24" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>SNN</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>28.15</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>0.002885714285714285</v>
+      </c>
+      <c r="D25" s="4" t="n">
+        <v>0.4761904761904762</v>
+      </c>
+      <c r="E25" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>TT</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>177.03</v>
+      </c>
+      <c r="C26" s="4" t="n">
+        <v>0.002842857142857143</v>
+      </c>
+      <c r="D26" s="4" t="n">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>6.32</v>
+      </c>
+      <c r="C27" s="4" t="n">
+        <v>0.00258095238095238</v>
+      </c>
+      <c r="D27" s="4" t="n">
+        <v>0.6190476190476191</v>
+      </c>
+      <c r="E27" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>PRU</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>103.5</v>
+      </c>
+      <c r="C28" s="4" t="n">
+        <v>0.002519047619047619</v>
+      </c>
+      <c r="D28" s="4" t="n">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>BP</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>36.32</v>
+      </c>
+      <c r="C29" s="4" t="n">
+        <v>0.0024</v>
+      </c>
+      <c r="D29" s="4" t="n">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>BAB</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>27.01</v>
+      </c>
+      <c r="C30" s="4" t="n">
+        <v>0.002366666666666667</v>
+      </c>
+      <c r="D30" s="4" t="n">
+        <v>0.5238095238095237</v>
+      </c>
+      <c r="E30" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>CNA</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>43.15</v>
+      </c>
+      <c r="C31" s="4" t="n">
+        <v>0.001571428571428571</v>
+      </c>
+      <c r="D31" s="4" t="n">
+        <v>0.4285714285714285</v>
+      </c>
+      <c r="E31" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>TSCO</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>225.67</v>
+      </c>
+      <c r="C32" s="4" t="n">
+        <v>0.001428571428571428</v>
+      </c>
+      <c r="D32" s="4" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CPI</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>25.3327</v>
+      </c>
+      <c r="C33" s="4" t="n">
+        <v>0.001142857142857143</v>
+      </c>
+      <c r="D33" s="4" t="n">
+        <v>0.4285714285714285</v>
+      </c>
+      <c r="E33" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>PSO</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>11.36</v>
+      </c>
+      <c r="C34" s="4" t="n">
+        <v>0.0009476190476190475</v>
+      </c>
+      <c r="D34" s="4" t="n">
+        <v>0.5238095238095237</v>
+      </c>
+      <c r="E34" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>GSK</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>35.3</v>
+      </c>
+      <c r="C35" s="4" t="n">
+        <v>0.0007428571428571431</v>
+      </c>
+      <c r="D35" s="4" t="n">
+        <v>0.5238095238095237</v>
+      </c>
+      <c r="E35" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>SMIN</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>50.73</v>
+      </c>
+      <c r="C36" s="4" t="n">
+        <v>-0.0006238095238095236</v>
+      </c>
+      <c r="D36" s="4" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>BG</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>97.59999999999999</v>
+      </c>
+      <c r="C37" s="4" t="n">
+        <v>-0.0007571428571428568</v>
+      </c>
+      <c r="D37" s="4" t="n">
+        <v>0.4761904761904762</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>AZN</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>65.53</v>
+      </c>
+      <c r="C38" s="4" t="n">
+        <v>-0.001380952380952381</v>
+      </c>
+      <c r="D38" s="4" t="n">
+        <v>0.4761904761904762</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>BTI</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>37.55</v>
+      </c>
+      <c r="C39" s="4" t="n">
+        <v>-0.003142857142857143</v>
+      </c>
+      <c r="D39" s="4" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>PFC</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>24.65</v>
+      </c>
+      <c r="C40" s="4" t="n">
+        <v>-0.003300000000000001</v>
+      </c>
+      <c r="D40" s="4" t="n">
+        <v>0.5238095238095237</v>
+      </c>
+      <c r="E40" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
           <t>ADM</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B41" t="n">
         <v>83.63</v>
       </c>
-      <c r="C13" s="4" t="n">
+      <c r="C41" s="4" t="n">
         <v>-0.005233333333333331</v>
       </c>
-      <c r="D13" s="4" t="n">
+      <c r="D41" s="4" t="n">
         <v>0.3333333333333333</v>
       </c>
-      <c r="E13" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" s="4" t="n"/>
-      <c r="D14" s="4" t="n"/>
-    </row>
-    <row r="15">
-      <c r="C15" s="4" t="n"/>
-      <c r="D15" s="4" t="n"/>
-    </row>
-    <row r="16">
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="4" t="n"/>
-    </row>
-    <row r="17">
-      <c r="C17" s="4" t="n"/>
-      <c r="D17" s="4" t="n"/>
-    </row>
-    <row r="18">
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="4" t="n"/>
-    </row>
-    <row r="19">
-      <c r="C19" s="4" t="n"/>
-      <c r="D19" s="4" t="n"/>
-    </row>
-    <row r="20">
-      <c r="C20" s="4" t="n"/>
-      <c r="D20" s="4" t="n"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="4" t="n"/>
-      <c r="D21" s="4" t="n"/>
-    </row>
-    <row r="22">
-      <c r="C22" s="4" t="n"/>
-      <c r="D22" s="4" t="n"/>
-    </row>
-    <row r="23">
-      <c r="C23" s="4" t="n"/>
-      <c r="D23" s="4" t="n"/>
-    </row>
-    <row r="24">
-      <c r="C24" s="4" t="n"/>
-      <c r="D24" s="4" t="n"/>
-    </row>
-    <row r="25">
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="4" t="n"/>
-    </row>
-    <row r="26">
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="4" t="n"/>
-    </row>
-    <row r="27">
-      <c r="C27" s="4" t="n"/>
-      <c r="D27" s="4" t="n"/>
-    </row>
-    <row r="28">
-      <c r="C28" s="4" t="n"/>
-      <c r="D28" s="4" t="n"/>
-    </row>
-    <row r="29">
-      <c r="C29" s="4" t="n"/>
-      <c r="D29" s="4" t="n"/>
-    </row>
-    <row r="30">
-      <c r="C30" s="4" t="n"/>
-      <c r="D30" s="4" t="n"/>
-    </row>
-    <row r="31">
-      <c r="C31" s="4" t="n"/>
-      <c r="D31" s="4" t="n"/>
-    </row>
-    <row r="32">
-      <c r="C32" s="4" t="n"/>
-      <c r="D32" s="4" t="n"/>
-    </row>
-    <row r="33">
-      <c r="C33" s="4" t="n"/>
-      <c r="D33" s="4" t="n"/>
-    </row>
-    <row r="34">
-      <c r="C34" s="4" t="n"/>
-      <c r="D34" s="4" t="n"/>
+      <c r="E41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="C42" s="4" t="n"/>
+      <c r="D42" s="4" t="n"/>
+    </row>
+    <row r="43">
+      <c r="C43" s="4" t="n"/>
+      <c r="D43" s="4" t="n"/>
+    </row>
+    <row r="44">
+      <c r="C44" s="4" t="n"/>
+      <c r="D44" s="4" t="n"/>
+    </row>
+    <row r="45">
+      <c r="C45" s="4" t="n"/>
+      <c r="D45" s="4" t="n"/>
+    </row>
+    <row r="46">
+      <c r="C46" s="4" t="n"/>
+      <c r="D46" s="4" t="n"/>
+    </row>
+    <row r="47">
+      <c r="C47" s="4" t="n"/>
+      <c r="D47" s="4" t="n"/>
+    </row>
+    <row r="48">
+      <c r="C48" s="4" t="n"/>
+      <c r="D48" s="4" t="n"/>
+    </row>
+    <row r="49">
+      <c r="C49" s="4" t="n"/>
+      <c r="D49" s="4" t="n"/>
+    </row>
+    <row r="50">
+      <c r="C50" s="4" t="n"/>
+      <c r="D50" s="4" t="n"/>
+    </row>
+    <row r="51">
+      <c r="C51" s="4" t="n"/>
+      <c r="D51" s="4" t="n"/>
+    </row>
+    <row r="52">
+      <c r="C52" s="4" t="n"/>
+      <c r="D52" s="4" t="n"/>
+    </row>
+    <row r="53">
+      <c r="C53" s="4" t="n"/>
+      <c r="D53" s="4" t="n"/>
+    </row>
+    <row r="54">
+      <c r="C54" s="4" t="n"/>
+      <c r="D54" s="4" t="n"/>
+    </row>
+    <row r="55">
+      <c r="C55" s="4" t="n"/>
+      <c r="D55" s="4" t="n"/>
+    </row>
+    <row r="56">
+      <c r="C56" s="4" t="n"/>
+      <c r="D56" s="4" t="n"/>
+    </row>
+    <row r="57">
+      <c r="C57" s="4" t="n"/>
+      <c r="D57" s="4" t="n"/>
+    </row>
+    <row r="58">
+      <c r="C58" s="4" t="n"/>
+      <c r="D58" s="4" t="n"/>
+    </row>
+    <row r="59">
+      <c r="C59" s="4" t="n"/>
+      <c r="D59" s="4" t="n"/>
+    </row>
+    <row r="60">
+      <c r="C60" s="4" t="n"/>
+      <c r="D60" s="4" t="n"/>
+    </row>
+    <row r="61">
+      <c r="C61" s="4" t="n"/>
+      <c r="D61" s="4" t="n"/>
+    </row>
+    <row r="62">
+      <c r="C62" s="4" t="n"/>
+      <c r="D62" s="4" t="n"/>
+    </row>
+    <row r="63">
+      <c r="C63" s="4" t="n"/>
+      <c r="D63" s="4" t="n"/>
+    </row>
+    <row r="64">
+      <c r="C64" s="4" t="n"/>
+      <c r="D64" s="4" t="n"/>
+    </row>
+    <row r="65">
+      <c r="C65" s="4" t="n"/>
+      <c r="D65" s="4" t="n"/>
+    </row>
+    <row r="66">
+      <c r="C66" s="4" t="n"/>
+      <c r="D66" s="4" t="n"/>
+    </row>
+    <row r="67">
+      <c r="C67" s="4" t="n"/>
+      <c r="D67" s="4" t="n"/>
+    </row>
+    <row r="68">
+      <c r="C68" s="4" t="n"/>
+      <c r="D68" s="4" t="n"/>
+    </row>
+    <row r="69">
+      <c r="C69" s="4" t="n"/>
+      <c r="D69" s="4" t="n"/>
+    </row>
+    <row r="70">
+      <c r="C70" s="4" t="n"/>
+      <c r="D70" s="4" t="n"/>
+    </row>
+    <row r="71">
+      <c r="C71" s="4" t="n"/>
+      <c r="D71" s="4" t="n"/>
+    </row>
+    <row r="72">
+      <c r="C72" s="4" t="n"/>
+      <c r="D72" s="4" t="n"/>
+    </row>
+    <row r="73">
+      <c r="C73" s="4" t="n"/>
+      <c r="D73" s="4" t="n"/>
+    </row>
+    <row r="74">
+      <c r="C74" s="4" t="n"/>
+      <c r="D74" s="4" t="n"/>
+    </row>
+    <row r="75">
+      <c r="C75" s="4" t="n"/>
+      <c r="D75" s="4" t="n"/>
+    </row>
+    <row r="76">
+      <c r="C76" s="4" t="n"/>
+      <c r="D76" s="4" t="n"/>
+    </row>
+    <row r="77">
+      <c r="C77" s="4" t="n"/>
+      <c r="D77" s="4" t="n"/>
+    </row>
+    <row r="78">
+      <c r="C78" s="4" t="n"/>
+      <c r="D78" s="4" t="n"/>
+    </row>
+    <row r="79">
+      <c r="C79" s="4" t="n"/>
+      <c r="D79" s="4" t="n"/>
+    </row>
+    <row r="80">
+      <c r="C80" s="4" t="n"/>
+      <c r="D80" s="4" t="n"/>
+    </row>
+    <row r="81">
+      <c r="C81" s="4" t="n"/>
+      <c r="D81" s="4" t="n"/>
+    </row>
+    <row r="82">
+      <c r="C82" s="4" t="n"/>
+      <c r="D82" s="4" t="n"/>
+    </row>
+    <row r="83">
+      <c r="C83" s="4" t="n"/>
+      <c r="D83" s="4" t="n"/>
+    </row>
+    <row r="84">
+      <c r="C84" s="4" t="n"/>
+      <c r="D84" s="4" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>